<commit_message>
completed jupyter notebook and added a full working module
</commit_message>
<xml_diff>
--- a/data/boolean-50PC.xlsx
+++ b/data/boolean-50PC.xlsx
@@ -1,54 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
+  <workbookProtection/>
   <bookViews>
-    <workbookView activeTab="0"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
-</file>
-
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="11">
-  <si>
-    <t>INITIAL</t>
-  </si>
-  <si>
-    <t>USA-LOW</t>
-  </si>
-  <si>
-    <t>GERMANY-LOW</t>
-  </si>
-  <si>
-    <t>JAPAN-LOW</t>
-  </si>
-  <si>
-    <t>BRAZIL-LOW</t>
-  </si>
-  <si>
-    <t>INDIA-LOW</t>
-  </si>
-  <si>
-    <t>USA-HIGH</t>
-  </si>
-  <si>
-    <t>GERMANY-HIGH</t>
-  </si>
-  <si>
-    <t>JAPAN-HIGH</t>
-  </si>
-  <si>
-    <t>BRAZIL-HIGH</t>
-  </si>
-  <si>
-    <t>INDIA-HIGH</t>
-  </si>
-</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -87,22 +50,89 @@
       <right style="thin"/>
       <top style="thin"/>
       <bottom style="thin"/>
-      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf applyAlignment="1" borderId="1" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" hidden="0" name="Normal" xfId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
   </cellStyles>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -403,9 +433,11 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:51">
-      <c r="B1" s="1" t="s">
-        <v>0</v>
+    <row r="1">
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>INITIAL</t>
+        </is>
       </c>
       <c r="C1" s="1" t="n">
         <v>1</v>
@@ -555,9 +587,11 @@
         <v>49</v>
       </c>
     </row>
-    <row r="2" spans="1:51">
-      <c r="A2" s="1" t="s">
-        <v>1</v>
+    <row r="2">
+      <c r="A2" s="1" t="inlineStr">
+        <is>
+          <t>USA-LOW</t>
+        </is>
       </c>
       <c r="B2" t="n">
         <v>0</v>
@@ -710,9 +744,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:51">
-      <c r="A3" s="1" t="s">
-        <v>2</v>
+    <row r="3">
+      <c r="A3" s="1" t="inlineStr">
+        <is>
+          <t>GERMANY-LOW</t>
+        </is>
       </c>
       <c r="B3" t="n">
         <v>0</v>
@@ -751,7 +787,7 @@
         <v>0</v>
       </c>
       <c r="N3" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O3" t="n">
         <v>0</v>
@@ -775,7 +811,7 @@
         <v>0</v>
       </c>
       <c r="V3" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W3" t="n">
         <v>0</v>
@@ -784,7 +820,7 @@
         <v>0</v>
       </c>
       <c r="Y3" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z3" t="n">
         <v>0</v>
@@ -796,7 +832,7 @@
         <v>0</v>
       </c>
       <c r="AC3" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AD3" t="n">
         <v>0</v>
@@ -805,7 +841,7 @@
         <v>0</v>
       </c>
       <c r="AF3" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AG3" t="n">
         <v>0</v>
@@ -817,13 +853,13 @@
         <v>0</v>
       </c>
       <c r="AJ3" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AK3" t="n">
         <v>0</v>
       </c>
       <c r="AL3" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AM3" t="n">
         <v>0</v>
@@ -844,7 +880,7 @@
         <v>0</v>
       </c>
       <c r="AS3" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AT3" t="n">
         <v>0</v>
@@ -865,9 +901,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:51">
-      <c r="A4" s="1" t="s">
-        <v>3</v>
+    <row r="4">
+      <c r="A4" s="1" t="inlineStr">
+        <is>
+          <t>JAPAN-LOW</t>
+        </is>
       </c>
       <c r="B4" t="n">
         <v>0</v>
@@ -885,7 +923,7 @@
         <v>0</v>
       </c>
       <c r="G4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H4" t="n">
         <v>0</v>
@@ -924,7 +962,7 @@
         <v>0</v>
       </c>
       <c r="T4" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U4" t="n">
         <v>0</v>
@@ -933,19 +971,19 @@
         <v>0</v>
       </c>
       <c r="W4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y4" t="n">
         <v>0</v>
       </c>
       <c r="Z4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AB4" t="n">
         <v>0</v>
@@ -969,7 +1007,7 @@
         <v>0</v>
       </c>
       <c r="AI4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AJ4" t="n">
         <v>0</v>
@@ -996,7 +1034,7 @@
         <v>0</v>
       </c>
       <c r="AR4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AS4" t="n">
         <v>0</v>
@@ -1020,18 +1058,20 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:51">
-      <c r="A5" s="1" t="s">
-        <v>4</v>
+    <row r="5">
+      <c r="A5" s="1" t="inlineStr">
+        <is>
+          <t>BRAZIL-LOW</t>
+        </is>
       </c>
       <c r="B5" t="n">
         <v>0</v>
       </c>
       <c r="C5" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D5" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E5" t="n">
         <v>0</v>
@@ -1040,19 +1080,19 @@
         <v>0</v>
       </c>
       <c r="G5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J5" t="n">
         <v>0</v>
       </c>
       <c r="K5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L5" t="n">
         <v>0</v>
@@ -1070,28 +1110,28 @@
         <v>1</v>
       </c>
       <c r="Q5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R5" t="n">
         <v>0</v>
       </c>
       <c r="S5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T5" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V5" t="n">
         <v>1</v>
       </c>
       <c r="W5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y5" t="n">
         <v>1</v>
@@ -1100,34 +1140,34 @@
         <v>1</v>
       </c>
       <c r="AA5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AB5" t="n">
         <v>0</v>
       </c>
       <c r="AC5" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AD5" t="n">
         <v>0</v>
       </c>
       <c r="AE5" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AF5" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AG5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AH5" t="n">
         <v>1</v>
       </c>
       <c r="AI5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AJ5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AK5" t="n">
         <v>0</v>
@@ -1136,13 +1176,13 @@
         <v>1</v>
       </c>
       <c r="AM5" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AN5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AO5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AP5" t="n">
         <v>1</v>
@@ -1154,19 +1194,19 @@
         <v>1</v>
       </c>
       <c r="AS5" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AT5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AU5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AV5" t="n">
         <v>1</v>
       </c>
       <c r="AW5" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AX5" t="n">
         <v>0</v>
@@ -1175,9 +1215,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:51">
-      <c r="A6" s="1" t="s">
-        <v>5</v>
+    <row r="6">
+      <c r="A6" s="1" t="inlineStr">
+        <is>
+          <t>INDIA-LOW</t>
+        </is>
       </c>
       <c r="B6" t="n">
         <v>1</v>
@@ -1192,10 +1234,10 @@
         <v>1</v>
       </c>
       <c r="F6" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H6" t="n">
         <v>1</v>
@@ -1204,7 +1246,7 @@
         <v>1</v>
       </c>
       <c r="J6" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K6" t="n">
         <v>1</v>
@@ -1219,7 +1261,7 @@
         <v>1</v>
       </c>
       <c r="O6" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P6" t="n">
         <v>1</v>
@@ -1234,7 +1276,7 @@
         <v>1</v>
       </c>
       <c r="T6" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U6" t="n">
         <v>1</v>
@@ -1258,7 +1300,7 @@
         <v>1</v>
       </c>
       <c r="AB6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AC6" t="n">
         <v>1</v>
@@ -1267,10 +1309,10 @@
         <v>1</v>
       </c>
       <c r="AE6" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AF6" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AG6" t="n">
         <v>1</v>
@@ -1279,13 +1321,13 @@
         <v>1</v>
       </c>
       <c r="AI6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AJ6" t="n">
         <v>1</v>
       </c>
       <c r="AK6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AL6" t="n">
         <v>1</v>
@@ -1309,7 +1351,7 @@
         <v>1</v>
       </c>
       <c r="AS6" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AT6" t="n">
         <v>1</v>
@@ -1330,9 +1372,11 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:51">
-      <c r="A7" s="1" t="s">
-        <v>6</v>
+    <row r="7">
+      <c r="A7" s="1" t="inlineStr">
+        <is>
+          <t>USA-HIGH</t>
+        </is>
       </c>
       <c r="B7" t="n">
         <v>0</v>
@@ -1353,7 +1397,7 @@
         <v>0</v>
       </c>
       <c r="H7" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I7" t="n">
         <v>0</v>
@@ -1395,7 +1439,7 @@
         <v>0</v>
       </c>
       <c r="V7" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W7" t="n">
         <v>0</v>
@@ -1404,10 +1448,10 @@
         <v>0</v>
       </c>
       <c r="Y7" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z7" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AA7" t="n">
         <v>0</v>
@@ -1443,7 +1487,7 @@
         <v>0</v>
       </c>
       <c r="AL7" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AM7" t="n">
         <v>0</v>
@@ -1473,21 +1517,23 @@
         <v>0</v>
       </c>
       <c r="AV7" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AW7" t="n">
         <v>0</v>
       </c>
       <c r="AX7" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AY7" t="n">
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:51">
-      <c r="A8" s="1" t="s">
-        <v>7</v>
+    <row r="8">
+      <c r="A8" s="1" t="inlineStr">
+        <is>
+          <t>GERMANY-HIGH</t>
+        </is>
       </c>
       <c r="B8" t="n">
         <v>0</v>
@@ -1508,10 +1554,10 @@
         <v>0</v>
       </c>
       <c r="H8" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I8" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J8" t="n">
         <v>0</v>
@@ -1523,10 +1569,10 @@
         <v>0</v>
       </c>
       <c r="M8" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N8" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O8" t="n">
         <v>0</v>
@@ -1535,7 +1581,7 @@
         <v>0</v>
       </c>
       <c r="Q8" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R8" t="n">
         <v>0</v>
@@ -1553,13 +1599,13 @@
         <v>0</v>
       </c>
       <c r="W8" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X8" t="n">
         <v>0</v>
       </c>
       <c r="Y8" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z8" t="n">
         <v>0</v>
@@ -1589,7 +1635,7 @@
         <v>0</v>
       </c>
       <c r="AI8" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AJ8" t="n">
         <v>0</v>
@@ -1610,7 +1656,7 @@
         <v>0</v>
       </c>
       <c r="AP8" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AQ8" t="n">
         <v>0</v>
@@ -1634,15 +1680,17 @@
         <v>0</v>
       </c>
       <c r="AX8" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AY8" t="n">
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:51">
-      <c r="A9" s="1" t="s">
-        <v>8</v>
+    <row r="9">
+      <c r="A9" s="1" t="inlineStr">
+        <is>
+          <t>JAPAN-HIGH</t>
+        </is>
       </c>
       <c r="B9" t="n">
         <v>1</v>
@@ -1651,13 +1699,13 @@
         <v>1</v>
       </c>
       <c r="D9" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E9" t="n">
         <v>1</v>
       </c>
       <c r="F9" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G9" t="n">
         <v>1</v>
@@ -1669,10 +1717,10 @@
         <v>1</v>
       </c>
       <c r="J9" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K9" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L9" t="n">
         <v>1</v>
@@ -1690,10 +1738,10 @@
         <v>1</v>
       </c>
       <c r="Q9" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R9" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S9" t="n">
         <v>0</v>
@@ -1702,7 +1750,7 @@
         <v>1</v>
       </c>
       <c r="U9" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V9" t="n">
         <v>1</v>
@@ -1720,13 +1768,13 @@
         <v>1</v>
       </c>
       <c r="AA9" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AB9" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AC9" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AD9" t="n">
         <v>1</v>
@@ -1735,7 +1783,7 @@
         <v>1</v>
       </c>
       <c r="AF9" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AG9" t="n">
         <v>1</v>
@@ -1753,7 +1801,7 @@
         <v>1</v>
       </c>
       <c r="AL9" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AM9" t="n">
         <v>1</v>
@@ -1762,42 +1810,44 @@
         <v>1</v>
       </c>
       <c r="AO9" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AP9" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AQ9" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AR9" t="n">
         <v>1</v>
       </c>
       <c r="AS9" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AT9" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AU9" t="n">
         <v>1</v>
       </c>
       <c r="AV9" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AW9" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AX9" t="n">
         <v>1</v>
       </c>
       <c r="AY9" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:51">
-      <c r="A10" s="1" t="s">
-        <v>9</v>
+    <row r="10">
+      <c r="A10" s="1" t="inlineStr">
+        <is>
+          <t>BRAZIL-HIGH</t>
+        </is>
       </c>
       <c r="B10" t="n">
         <v>1</v>
@@ -1851,7 +1901,7 @@
         <v>1</v>
       </c>
       <c r="S10" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T10" t="n">
         <v>1</v>
@@ -1875,7 +1925,7 @@
         <v>1</v>
       </c>
       <c r="AA10" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AB10" t="n">
         <v>1</v>
@@ -1908,7 +1958,7 @@
         <v>1</v>
       </c>
       <c r="AL10" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AM10" t="n">
         <v>1</v>
@@ -1920,10 +1970,10 @@
         <v>1</v>
       </c>
       <c r="AP10" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AQ10" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AR10" t="n">
         <v>1</v>
@@ -1938,7 +1988,7 @@
         <v>1</v>
       </c>
       <c r="AV10" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AW10" t="n">
         <v>1</v>
@@ -1950,9 +2000,11 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:51">
-      <c r="A11" s="1" t="s">
-        <v>10</v>
+    <row r="11">
+      <c r="A11" s="1" t="inlineStr">
+        <is>
+          <t>INDIA-HIGH</t>
+        </is>
       </c>
       <c r="B11" t="n">
         <v>1</v>
@@ -2078,7 +2130,7 @@
         <v>1</v>
       </c>
       <c r="AQ11" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AR11" t="n">
         <v>1</v>
@@ -2106,6 +2158,6 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>